<commit_message>
Reworked section 3. Added open set figure.
</commit_message>
<xml_diff>
--- a/tab/detectionEval.xlsx
+++ b/tab/detectionEval.xlsx
@@ -109,6 +109,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FF813FB7"/>
       <color rgb="FF0066FF"/>
     </mruColors>
   </colors>
@@ -154,7 +155,7 @@
           <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>2FRCNN, public+LitW</c:v>
+            <c:v>brand agnostic, public+LitW</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="12700" cap="rnd">
@@ -786,7 +787,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>2FRCNN, public</c:v>
+            <c:v>brand agnostic, public</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="12700" cap="rnd">
@@ -1423,7 +1424,7 @@
           <c:spPr>
             <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:srgbClr val="813FB7"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2054,11 +2055,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65996480"/>
-        <c:axId val="66628416"/>
+        <c:axId val="596838080"/>
+        <c:axId val="596841536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65996480"/>
+        <c:axId val="596838080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2145,12 +2146,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66628416"/>
+        <c:crossAx val="596841536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66628416"/>
+        <c:axId val="596841536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
@@ -2227,7 +2228,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65996480"/>
+        <c:crossAx val="596838080"/>
         <c:crossesAt val="1.0000000000000002E-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2245,10 +2246,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.19843749999999999"/>
-          <c:y val="3.4046759259259263E-2"/>
-          <c:w val="0.55344340277777782"/>
-          <c:h val="0.20871203703703706"/>
+          <c:x val="0.18079861111111112"/>
+          <c:y val="4.5806018518518517E-2"/>
+          <c:w val="0.62840868055555554"/>
+          <c:h val="0.16755462962962964"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3145,7 +3146,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3156,7 +3157,7 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>